<commit_message>
compound names are now the same as in xml file
</commit_message>
<xml_diff>
--- a/opiate/data/qa.xlsx
+++ b/opiate/data/qa.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>compound</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Hydrocodone</t>
   </si>
   <si>
-    <t>6-monoacetylmorphine</t>
-  </si>
-  <si>
     <t>Norfentanyl</t>
   </si>
   <si>
@@ -90,18 +87,6 @@
     <t>Methadone</t>
   </si>
   <si>
-    <t>Morphine-3-glucuronide</t>
-  </si>
-  <si>
-    <t>Morphine-6-glucuronide</t>
-  </si>
-  <si>
-    <t>Oxymorphone glucuronide</t>
-  </si>
-  <si>
-    <t>Hydromorphone glucuronide</t>
-  </si>
-  <si>
     <t>Codeine-6-glucuronide</t>
   </si>
   <si>
@@ -118,13 +103,31 @@
   </si>
   <si>
     <t>rel_reten_high</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>6-Monoacetylmorphine</t>
+  </si>
+  <si>
+    <t>Oxymorphone Glucuronide</t>
+  </si>
+  <si>
+    <t>Morphine-3-B-D-glucuronide</t>
+  </si>
+  <si>
+    <t>Morphine-6-B-D-glucuronide</t>
+  </si>
+  <si>
+    <t>Hydromorphone-3-B-D-glucuronide</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +259,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -558,7 +577,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -601,12 +620,32 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -635,11 +674,31 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="43" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="45" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="47" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="49" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="51" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="53" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="55" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="57" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="59" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="61" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="42" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="44" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="46" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="50" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="52" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="54" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="56" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="58" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="60" builtinId="8" hidden="1"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -947,724 +1006,804 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M21"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J27" sqref="J27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>6</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="N1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>1.1160000000000001</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>1.3640000000000001</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>0.995</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>1.0349999999999999</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>10</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>1000</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>47</v>
       </c>
-      <c r="I2">
-        <v>8</v>
-      </c>
-      <c r="J2" s="1">
+      <c r="J2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="1">
         <v>7000</v>
       </c>
     </row>
-    <row r="3" spans="1:13">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>10</v>
       </c>
       <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
         <v>0.34</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>0.47</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>0.98599999999999999</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>1.026</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>10</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>1000</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>48</v>
       </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3" s="1">
+      <c r="J3">
+        <v>8</v>
+      </c>
+      <c r="K3" s="1">
         <v>31000</v>
       </c>
     </row>
-    <row r="4" spans="1:13">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
         <v>1.56</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>0.98099999999999998</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>1.0209999999999999</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>1000</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>132</v>
       </c>
-      <c r="I4">
-        <v>8</v>
-      </c>
-      <c r="J4" s="1">
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4" s="1">
         <v>20000</v>
       </c>
     </row>
-    <row r="5" spans="1:13">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>12</v>
       </c>
       <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
         <v>1.75</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2.4700000000000002</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>0.98699999999999999</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1.0269999999999999</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>10</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>1000</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>29</v>
       </c>
-      <c r="I5">
-        <v>8</v>
-      </c>
-      <c r="J5" s="1">
+      <c r="J5">
+        <v>8</v>
+      </c>
+      <c r="K5" s="1">
         <v>10000</v>
       </c>
     </row>
-    <row r="6" spans="1:13">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>13</v>
       </c>
       <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
         <v>0.22600000000000001</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>0.35399999999999998</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>0.98799999999999999</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>1.028</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>1000</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>64</v>
       </c>
-      <c r="I6">
-        <v>8</v>
-      </c>
-      <c r="J6" s="1">
+      <c r="J6">
+        <v>8</v>
+      </c>
+      <c r="K6" s="1">
         <v>25000</v>
       </c>
     </row>
-    <row r="7" spans="1:13">
+    <row r="7" spans="1:14">
       <c r="A7" t="s">
         <v>14</v>
       </c>
       <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
         <v>2.34</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>3.9</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>0.98199999999999998</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>1.022</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>10</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>1000</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>95</v>
       </c>
-      <c r="I7">
-        <v>8</v>
-      </c>
-      <c r="J7" s="1">
+      <c r="J7">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1">
         <v>64000</v>
       </c>
     </row>
-    <row r="8" spans="1:13">
+    <row r="8" spans="1:14">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <v>1.6</v>
+      </c>
+      <c r="D8">
+        <v>1.84</v>
+      </c>
+      <c r="E8">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="F8">
+        <v>1.024</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>1000</v>
+      </c>
+      <c r="I8">
+        <v>122</v>
+      </c>
+      <c r="J8">
+        <v>8</v>
+      </c>
+      <c r="K8" s="1">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>1.6</v>
-      </c>
-      <c r="C8">
-        <v>1.84</v>
-      </c>
-      <c r="D8">
-        <v>0.98399999999999999</v>
-      </c>
-      <c r="E8">
-        <v>1.024</v>
-      </c>
-      <c r="F8">
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <v>14.292999999999999</v>
+      </c>
+      <c r="D9">
+        <v>20.146999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.98199999999999998</v>
+      </c>
+      <c r="F9">
+        <v>1.022</v>
+      </c>
+      <c r="G9">
         <v>10</v>
       </c>
-      <c r="G8">
+      <c r="H9">
         <v>1000</v>
       </c>
-      <c r="H8">
-        <v>122</v>
-      </c>
-      <c r="I8">
-        <v>8</v>
-      </c>
-      <c r="J8" s="1">
-        <v>13000</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" t="s">
+      <c r="I9">
+        <v>343</v>
+      </c>
+      <c r="J9">
+        <v>8</v>
+      </c>
+      <c r="K9" s="1">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>14.292999999999999</v>
-      </c>
-      <c r="C9">
-        <v>20.146999999999998</v>
-      </c>
-      <c r="D9">
-        <v>0.98199999999999998</v>
-      </c>
-      <c r="E9">
-        <v>1.022</v>
-      </c>
-      <c r="F9">
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>3.3029999999999999</v>
+      </c>
+      <c r="D10">
+        <v>4.0369999999999999</v>
+      </c>
+      <c r="E10">
+        <v>0.98</v>
+      </c>
+      <c r="F10">
+        <v>1.02</v>
+      </c>
+      <c r="G10">
         <v>10</v>
       </c>
-      <c r="G9">
+      <c r="H10">
         <v>1000</v>
       </c>
-      <c r="H9">
-        <v>343</v>
-      </c>
-      <c r="I9">
-        <v>8</v>
-      </c>
-      <c r="J9" s="1">
+      <c r="I10">
+        <v>164</v>
+      </c>
+      <c r="J10">
+        <v>8</v>
+      </c>
+      <c r="K10" s="1">
+        <v>104000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <v>1.075</v>
+      </c>
+      <c r="D11">
+        <v>1.4850000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F11">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="G11">
+        <v>10</v>
+      </c>
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11">
+        <v>134</v>
+      </c>
+      <c r="J11">
+        <v>8</v>
+      </c>
+      <c r="K11" s="1">
+        <v>87000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <v>0.65</v>
+      </c>
+      <c r="D12">
+        <v>1.67</v>
+      </c>
+      <c r="E12">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F12">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="G12">
+        <v>0.25</v>
+      </c>
+      <c r="H12">
+        <v>25</v>
+      </c>
+      <c r="I12">
+        <v>36</v>
+      </c>
+      <c r="J12">
+        <v>8</v>
+      </c>
+      <c r="K12" s="1">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>0.72799999999999998</v>
+      </c>
+      <c r="D13">
+        <v>1.212</v>
+      </c>
+      <c r="E13">
+        <v>0.98</v>
+      </c>
+      <c r="F13">
+        <v>1.02</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>1000</v>
+      </c>
+      <c r="I13">
+        <v>32</v>
+      </c>
+      <c r="J13">
+        <v>8</v>
+      </c>
+      <c r="K13" s="1">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <v>1.05</v>
+      </c>
+      <c r="D14">
+        <v>1.95</v>
+      </c>
+      <c r="E14">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F14">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>1000</v>
+      </c>
+      <c r="I14">
+        <v>295</v>
+      </c>
+      <c r="J14">
+        <v>8</v>
+      </c>
+      <c r="K14" s="1">
+        <v>48000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>0.18</v>
+      </c>
+      <c r="D15">
+        <v>0.22</v>
+      </c>
+      <c r="E15">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="F15">
+        <v>1.0209999999999999</v>
+      </c>
+      <c r="G15">
+        <v>10</v>
+      </c>
+      <c r="H15">
+        <v>1000</v>
+      </c>
+      <c r="I15">
+        <v>257</v>
+      </c>
+      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="K15" s="1">
+        <v>73000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>10.45</v>
+      </c>
+      <c r="D16">
+        <v>22.21</v>
+      </c>
+      <c r="E16">
+        <v>0.98599999999999999</v>
+      </c>
+      <c r="F16">
+        <v>1.026</v>
+      </c>
+      <c r="G16">
+        <v>100</v>
+      </c>
+      <c r="J16">
+        <v>8</v>
+      </c>
+      <c r="K16" s="1">
+        <v>8500</v>
+      </c>
+      <c r="L16">
+        <v>80</v>
+      </c>
+      <c r="M16">
+        <v>120</v>
+      </c>
+      <c r="N16">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <v>8.56</v>
+      </c>
+      <c r="D17">
+        <v>13.96</v>
+      </c>
+      <c r="E17">
+        <v>0.98</v>
+      </c>
+      <c r="F17">
+        <v>1.02</v>
+      </c>
+      <c r="G17">
+        <v>100</v>
+      </c>
+      <c r="J17">
+        <v>8</v>
+      </c>
+      <c r="K17" s="1">
+        <v>9000</v>
+      </c>
+      <c r="L17">
+        <v>80</v>
+      </c>
+      <c r="M17">
+        <v>120</v>
+      </c>
+      <c r="N17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <v>1.7949999999999999</v>
+      </c>
+      <c r="D18">
+        <v>5.3849999999999998</v>
+      </c>
+      <c r="E18">
+        <v>0.98</v>
+      </c>
+      <c r="F18">
+        <v>1.02</v>
+      </c>
+      <c r="G18">
+        <v>100</v>
+      </c>
+      <c r="J18">
+        <v>8</v>
+      </c>
+      <c r="L18">
+        <v>80</v>
+      </c>
+      <c r="M18">
+        <v>120</v>
+      </c>
+      <c r="N18">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <v>2.36</v>
+      </c>
+      <c r="D19">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="E19">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="F19">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="G19">
+        <v>100</v>
+      </c>
+      <c r="J19">
+        <v>8</v>
+      </c>
+      <c r="K19" s="1">
+        <v>3000</v>
+      </c>
+      <c r="L19">
+        <v>80</v>
+      </c>
+      <c r="M19">
+        <v>120</v>
+      </c>
+      <c r="N19">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>8.0039999999999996</v>
+      </c>
+      <c r="D20">
+        <v>15.196</v>
+      </c>
+      <c r="E20">
+        <v>0.97</v>
+      </c>
+      <c r="F20">
+        <v>1.03</v>
+      </c>
+      <c r="G20">
+        <v>100</v>
+      </c>
+      <c r="J20">
+        <v>8</v>
+      </c>
+      <c r="L20">
+        <v>80</v>
+      </c>
+      <c r="M20">
+        <v>120</v>
+      </c>
+      <c r="N20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>7.266</v>
+      </c>
+      <c r="D21">
+        <v>13.794</v>
+      </c>
+      <c r="E21">
+        <v>0.96030000000000004</v>
+      </c>
+      <c r="F21">
+        <v>1.0197000000000001</v>
+      </c>
+      <c r="G21">
+        <v>100</v>
+      </c>
+      <c r="J21">
+        <v>8</v>
+      </c>
+      <c r="K21" s="1">
         <v>36000</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10">
-        <v>3.3029999999999999</v>
-      </c>
-      <c r="C10">
-        <v>4.0369999999999999</v>
-      </c>
-      <c r="D10">
-        <v>0.98</v>
-      </c>
-      <c r="E10">
-        <v>1.02</v>
-      </c>
-      <c r="F10">
-        <v>10</v>
-      </c>
-      <c r="G10">
-        <v>1000</v>
-      </c>
-      <c r="H10">
-        <v>164</v>
-      </c>
-      <c r="I10">
-        <v>8</v>
-      </c>
-      <c r="J10" s="1">
-        <v>104000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" t="s">
-        <v>18</v>
-      </c>
-      <c r="B11">
-        <v>1.075</v>
-      </c>
-      <c r="C11">
-        <v>1.4850000000000001</v>
-      </c>
-      <c r="D11">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="E11">
-        <v>1.0209999999999999</v>
-      </c>
-      <c r="F11">
-        <v>10</v>
-      </c>
-      <c r="G11">
-        <v>1000</v>
-      </c>
-      <c r="H11">
-        <v>134</v>
-      </c>
-      <c r="I11">
-        <v>8</v>
-      </c>
-      <c r="J11" s="1">
-        <v>87000</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
-      <c r="B12">
-        <v>0.65</v>
-      </c>
-      <c r="C12">
-        <v>1.67</v>
-      </c>
-      <c r="D12">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="E12">
-        <v>1.0209999999999999</v>
-      </c>
-      <c r="F12">
-        <v>0.25</v>
-      </c>
-      <c r="G12">
-        <v>25</v>
-      </c>
-      <c r="H12">
-        <v>36</v>
-      </c>
-      <c r="I12">
-        <v>8</v>
-      </c>
-      <c r="J12" s="1">
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>0.72799999999999998</v>
-      </c>
-      <c r="C13">
-        <v>1.212</v>
-      </c>
-      <c r="D13">
-        <v>0.98</v>
-      </c>
-      <c r="E13">
-        <v>1.02</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>1000</v>
-      </c>
-      <c r="H13">
-        <v>32</v>
-      </c>
-      <c r="I13">
-        <v>8</v>
-      </c>
-      <c r="J13" s="1">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>1.05</v>
-      </c>
-      <c r="C14">
-        <v>1.95</v>
-      </c>
-      <c r="D14">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="E14">
-        <v>1.0209999999999999</v>
-      </c>
-      <c r="F14">
-        <v>10</v>
-      </c>
-      <c r="G14">
-        <v>1000</v>
-      </c>
-      <c r="H14">
-        <v>295</v>
-      </c>
-      <c r="I14">
-        <v>8</v>
-      </c>
-      <c r="J14" s="1">
-        <v>48000</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>0.18</v>
-      </c>
-      <c r="C15">
-        <v>0.22</v>
-      </c>
-      <c r="D15">
-        <v>0.98099999999999998</v>
-      </c>
-      <c r="E15">
-        <v>1.0209999999999999</v>
-      </c>
-      <c r="F15">
-        <v>10</v>
-      </c>
-      <c r="G15">
-        <v>1000</v>
-      </c>
-      <c r="H15">
-        <v>257</v>
-      </c>
-      <c r="I15">
-        <v>8</v>
-      </c>
-      <c r="J15" s="1">
-        <v>73000</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>10.45</v>
-      </c>
-      <c r="C16">
-        <v>22.21</v>
-      </c>
-      <c r="D16">
-        <v>0.98599999999999999</v>
-      </c>
-      <c r="E16">
-        <v>1.026</v>
-      </c>
-      <c r="F16">
+      <c r="L21">
+        <v>80</v>
+      </c>
+      <c r="M21">
+        <v>120</v>
+      </c>
+      <c r="N21">
         <v>100</v>
       </c>
-      <c r="I16">
-        <v>8</v>
-      </c>
-      <c r="J16" s="1">
-        <v>8500</v>
-      </c>
-      <c r="K16">
-        <v>80</v>
-      </c>
-      <c r="L16">
-        <v>120</v>
-      </c>
-      <c r="M16">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>8.56</v>
-      </c>
-      <c r="C17">
-        <v>13.96</v>
-      </c>
-      <c r="D17">
-        <v>0.98</v>
-      </c>
-      <c r="E17">
-        <v>1.02</v>
-      </c>
-      <c r="F17">
-        <v>100</v>
-      </c>
-      <c r="I17">
-        <v>8</v>
-      </c>
-      <c r="J17" s="1">
-        <v>9000</v>
-      </c>
-      <c r="K17">
-        <v>80</v>
-      </c>
-      <c r="L17">
-        <v>120</v>
-      </c>
-      <c r="M17">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18">
-        <v>2.36</v>
-      </c>
-      <c r="C18">
-        <v>4.4800000000000004</v>
-      </c>
-      <c r="D18">
-        <v>0.80800000000000005</v>
-      </c>
-      <c r="E18">
-        <v>0.85499999999999998</v>
-      </c>
-      <c r="F18">
-        <v>100</v>
-      </c>
-      <c r="I18">
-        <v>8</v>
-      </c>
-      <c r="J18" s="1">
-        <v>3000</v>
-      </c>
-      <c r="K18">
-        <v>80</v>
-      </c>
-      <c r="L18">
-        <v>120</v>
-      </c>
-      <c r="M18">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19">
-        <v>1.7949999999999999</v>
-      </c>
-      <c r="C19">
-        <v>5.3849999999999998</v>
-      </c>
-      <c r="D19">
-        <v>0.98</v>
-      </c>
-      <c r="E19">
-        <v>1.02</v>
-      </c>
-      <c r="F19">
-        <v>100</v>
-      </c>
-      <c r="I19">
-        <v>8</v>
-      </c>
-      <c r="K19">
-        <v>80</v>
-      </c>
-      <c r="L19">
-        <v>120</v>
-      </c>
-      <c r="M19">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="20" spans="1:13">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
-        <v>8.0039999999999996</v>
-      </c>
-      <c r="C20">
-        <v>15.196</v>
-      </c>
-      <c r="D20">
-        <v>0.97</v>
-      </c>
-      <c r="E20">
-        <v>1.03</v>
-      </c>
-      <c r="F20">
-        <v>100</v>
-      </c>
-      <c r="I20">
-        <v>8</v>
-      </c>
-      <c r="K20">
-        <v>80</v>
-      </c>
-      <c r="L20">
-        <v>120</v>
-      </c>
-      <c r="M20">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="21" spans="1:13">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21">
-        <v>7.266</v>
-      </c>
-      <c r="C21">
-        <v>13.794</v>
-      </c>
-      <c r="D21">
-        <v>0.96030000000000004</v>
-      </c>
-      <c r="E21">
-        <v>1.0197000000000001</v>
-      </c>
-      <c r="F21">
-        <v>100</v>
-      </c>
-      <c r="I21">
-        <v>8</v>
-      </c>
-      <c r="J21" s="1">
-        <v>36000</v>
-      </c>
-      <c r="K21">
-        <v>80</v>
-      </c>
-      <c r="L21">
-        <v>120</v>
-      </c>
-      <c r="M21">
-        <v>100</v>
-      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="K23"/>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="K24"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="K25"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="K26"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="K27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
* updated headers in qa.csv  * added unit tests for qa subcommand  * rudimentary container classes are in place
</commit_message>
<xml_diff>
--- a/opiate/data/qa.xlsx
+++ b/opiate/data/qa.xlsx
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
-    <t>compound</t>
-  </si>
-  <si>
     <t>amr_low</t>
   </si>
   <si>
@@ -105,9 +102,6 @@
     <t>rel_reten_high</t>
   </si>
   <si>
-    <t>id</t>
-  </si>
-  <si>
     <t>6-Monoacetylmorphine</t>
   </si>
   <si>
@@ -121,6 +115,12 @@
   </si>
   <si>
     <t>Hydromorphone-3-B-D-glucuronide</t>
+  </si>
+  <si>
+    <t>qa_compound</t>
+  </si>
+  <si>
+    <t>qa_id</t>
   </si>
 </sst>
 </file>
@@ -1008,14 +1008,12 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
@@ -1032,51 +1030,51 @@
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>1</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>2</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>3</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>6</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>7</v>
-      </c>
-      <c r="N1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:14">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1111,7 +1109,7 @@
     </row>
     <row r="3" spans="1:14">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B3">
         <v>2</v>
@@ -1146,7 +1144,7 @@
     </row>
     <row r="4" spans="1:14">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B4">
         <v>3</v>
@@ -1181,7 +1179,7 @@
     </row>
     <row r="5" spans="1:14">
       <c r="A5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1216,7 +1214,7 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -1251,7 +1249,7 @@
     </row>
     <row r="7" spans="1:14">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7">
         <v>6</v>
@@ -1286,7 +1284,7 @@
     </row>
     <row r="8" spans="1:14">
       <c r="A8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1321,7 +1319,7 @@
     </row>
     <row r="9" spans="1:14">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>8</v>
@@ -1356,7 +1354,7 @@
     </row>
     <row r="10" spans="1:14">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1391,7 +1389,7 @@
     </row>
     <row r="11" spans="1:14">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B11">
         <v>10</v>
@@ -1426,7 +1424,7 @@
     </row>
     <row r="12" spans="1:14">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B12">
         <v>11</v>
@@ -1461,7 +1459,7 @@
     </row>
     <row r="13" spans="1:14">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13">
         <v>12</v>
@@ -1496,7 +1494,7 @@
     </row>
     <row r="14" spans="1:14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14">
         <v>13</v>
@@ -1531,7 +1529,7 @@
     </row>
     <row r="15" spans="1:14">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15">
         <v>14</v>
@@ -1566,7 +1564,7 @@
     </row>
     <row r="16" spans="1:14">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B16">
         <v>15</v>
@@ -1604,7 +1602,7 @@
     </row>
     <row r="17" spans="1:14">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B17">
         <v>16</v>
@@ -1642,7 +1640,7 @@
     </row>
     <row r="18" spans="1:14">
       <c r="A18" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B18">
         <v>17</v>
@@ -1677,7 +1675,7 @@
     </row>
     <row r="19" spans="1:14">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B19">
         <v>18</v>
@@ -1715,7 +1713,7 @@
     </row>
     <row r="20" spans="1:14">
       <c r="A20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B20">
         <v>19</v>
@@ -1750,7 +1748,7 @@
     </row>
     <row r="21" spans="1:14">
       <c r="A21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B21">
         <v>20</v>

</xml_diff>

<commit_message>
change 'ion_ratio_average' to 'ion_ratio_agv' throughout
</commit_message>
<xml_diff>
--- a/opiate/data/qa.xlsx
+++ b/opiate/data/qa.xlsx
@@ -117,10 +117,10 @@
     <t>qa_id</t>
   </si>
   <si>
-    <t>ion_ratio_average</t>
-  </si>
-  <si>
     <t>ion_ratio_cv</t>
+  </si>
+  <si>
+    <t>ion_ratio_avg</t>
   </si>
 </sst>
 </file>
@@ -1009,7 +1009,7 @@
   <dimension ref="A1:N27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1038,10 +1038,10 @@
         <v>31</v>
       </c>
       <c r="C1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" t="s">
         <v>32</v>
-      </c>
-      <c r="D1" t="s">
-        <v>33</v>
       </c>
       <c r="E1" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
update target ratios for the glucuronides
</commit_message>
<xml_diff>
--- a/opiate/data/qa.xlsx
+++ b/opiate/data/qa.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="720" yWindow="315" windowWidth="21840" windowHeight="13440"/>
+    <workbookView xWindow="720" yWindow="320" windowWidth="21720" windowHeight="13440"/>
   </bookViews>
   <sheets>
     <sheet name="QA" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -644,10 +644,12 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="62">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1013,853 +1015,911 @@
   <dimension ref="A1:O27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="12.28515625" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" customWidth="1"/>
+    <col min="7" max="7" width="7.83203125" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18" customWidth="1"/>
+    <col min="15" max="15" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
+    <row r="2" spans="1:15">
+      <c r="A2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2" s="2">
         <v>1</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>1.2400000000000002</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>0.109</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>0.995</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>1.0349999999999999</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>10</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>1000</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>47</v>
       </c>
-      <c r="J2">
-        <v>8</v>
-      </c>
-      <c r="K2" s="1">
+      <c r="J2" s="2">
+        <v>8</v>
+      </c>
+      <c r="K2" s="3">
         <v>4000</v>
       </c>
-      <c r="O2">
+      <c r="L2" s="2"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:15">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="2">
         <v>2</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="2">
         <v>0.40500000000000003</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="2">
         <v>0.13900000000000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="2">
         <v>0.98599999999999999</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="2">
         <v>1.026</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="2">
         <v>10</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
         <v>1000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="2">
         <v>48</v>
       </c>
-      <c r="J3">
-        <v>8</v>
-      </c>
-      <c r="K3" s="1">
+      <c r="J3" s="2">
+        <v>8</v>
+      </c>
+      <c r="K3" s="3">
         <v>20000</v>
       </c>
-      <c r="O3">
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:15">
+      <c r="A4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>3</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>1.8800000000000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>0.158</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>0.98099999999999998</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>1.0209999999999999</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>10</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>1000</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>132</v>
       </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
-      <c r="K4" s="1">
+      <c r="J4" s="2">
+        <v>8</v>
+      </c>
+      <c r="K4" s="3">
         <v>8800</v>
       </c>
-      <c r="O4">
+      <c r="L4" s="2"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:15">
+      <c r="A5" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="2">
         <v>4</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="2">
         <v>2.1100000000000003</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="2">
         <v>0.17</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="2">
         <v>0.98699999999999999</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="2">
         <v>1.0269999999999999</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="2">
         <v>10</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="2">
         <v>1000</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="2">
         <v>29</v>
       </c>
-      <c r="J5">
-        <v>8</v>
-      </c>
-      <c r="K5" s="1">
+      <c r="J5" s="2">
+        <v>8</v>
+      </c>
+      <c r="K5" s="3">
         <v>6500</v>
       </c>
-      <c r="O5">
+      <c r="L5" s="2"/>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+      <c r="O5" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:15">
+      <c r="A6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="2">
         <v>5</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="2">
         <v>0.28999999999999998</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="2">
         <v>0.222</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="2">
         <v>0.98799999999999999</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="2">
         <v>1.028</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <v>10</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="2">
         <v>1000</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="2">
         <v>64</v>
       </c>
-      <c r="J6">
-        <v>8</v>
-      </c>
-      <c r="K6" s="1">
+      <c r="J6" s="2">
+        <v>8</v>
+      </c>
+      <c r="K6" s="3">
         <v>18000</v>
       </c>
-      <c r="O6">
+      <c r="L6" s="2"/>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+      <c r="O6" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:15">
+      <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="2">
         <v>6</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="2">
         <v>3.12</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>0.20799999999999999</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="2">
         <v>0.98199999999999998</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="2">
         <v>1.022</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <v>10</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="2">
         <v>1000</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="2">
         <v>95</v>
       </c>
-      <c r="J7">
-        <v>8</v>
-      </c>
-      <c r="K7" s="1">
+      <c r="J7" s="2">
+        <v>8</v>
+      </c>
+      <c r="K7" s="3">
         <v>51000</v>
       </c>
-      <c r="O7">
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="8" spans="1:15">
+      <c r="A8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="2">
         <v>7</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="2">
         <v>1.7200000000000002</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="2">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="2">
         <v>0.98399999999999999</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="2">
         <v>1.024</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="2">
         <v>5</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="2">
         <v>1000</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="2">
         <v>122</v>
       </c>
-      <c r="J8">
-        <v>8</v>
-      </c>
-      <c r="K8" s="1">
+      <c r="J8" s="2">
+        <v>8</v>
+      </c>
+      <c r="K8" s="3">
         <v>13000</v>
       </c>
-      <c r="O8">
+      <c r="L8" s="2"/>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+      <c r="O8" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="9" spans="1:15">
+      <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9">
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="2">
         <v>17.22</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="2">
         <v>0.16600000000000001</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="2">
         <v>0.98199999999999998</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="2">
         <v>1.022</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="2">
         <v>10</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>1000</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="2">
         <v>343</v>
       </c>
-      <c r="J9">
-        <v>8</v>
-      </c>
-      <c r="K9" s="1">
+      <c r="J9" s="2">
+        <v>8</v>
+      </c>
+      <c r="K9" s="3">
         <v>19000</v>
       </c>
-      <c r="O9">
+      <c r="L9" s="2"/>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+      <c r="O9" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:15">
+      <c r="A10" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="2">
         <v>9</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="2">
         <v>3.67</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="2">
         <v>0.06</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="2">
         <v>0.98</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="2">
         <v>1.02</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="2">
         <v>10</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="2">
         <v>1000</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="2">
         <v>164</v>
       </c>
-      <c r="J10">
-        <v>8</v>
-      </c>
-      <c r="K10" s="1">
+      <c r="J10" s="2">
+        <v>8</v>
+      </c>
+      <c r="K10" s="3">
         <v>93000</v>
       </c>
-      <c r="O10">
+      <c r="L10" s="2"/>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+      <c r="O10" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:15">
+      <c r="A11" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="2">
         <v>10</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="2">
         <v>1.28</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="2">
         <v>0.161</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="2">
         <v>0.98099999999999998</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="2">
         <v>1.0209999999999999</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="2">
         <v>10</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="2">
         <v>1000</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="2">
         <v>134</v>
       </c>
-      <c r="J11">
-        <v>8</v>
-      </c>
-      <c r="K11" s="1">
+      <c r="J11" s="2">
+        <v>8</v>
+      </c>
+      <c r="K11" s="3">
         <v>51000</v>
       </c>
-      <c r="O11">
+      <c r="L11" s="2"/>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+      <c r="O11" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:15">
+      <c r="A12" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B12">
+      <c r="B12" s="2">
         <v>11</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="2">
         <v>1.1599999999999999</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>0.39300000000000002</v>
       </c>
-      <c r="E12">
+      <c r="E12" s="2">
         <v>0.98099999999999998</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="2">
         <v>1.0209999999999999</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="2">
         <v>0.25</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="2">
         <v>25</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="2">
         <v>36</v>
       </c>
-      <c r="J12">
-        <v>8</v>
-      </c>
-      <c r="K12" s="1">
+      <c r="J12" s="2">
+        <v>8</v>
+      </c>
+      <c r="K12" s="3">
         <v>8000</v>
       </c>
-      <c r="O12">
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2">
         <v>0.62</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:15">
+      <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="2">
         <v>12</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="4">
         <v>0.56024894514767931</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="2">
         <v>0.189</v>
       </c>
-      <c r="E13">
+      <c r="E13" s="2">
         <v>0.98</v>
       </c>
-      <c r="F13">
+      <c r="F13" s="2">
         <v>1.02</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="2">
         <v>10</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="2">
         <v>1000</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="2">
         <v>32</v>
       </c>
-      <c r="J13">
-        <v>8</v>
-      </c>
-      <c r="K13" s="1">
+      <c r="J13" s="2">
+        <v>8</v>
+      </c>
+      <c r="K13" s="3">
         <v>3000</v>
       </c>
-      <c r="O13">
+      <c r="L13" s="2"/>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+      <c r="O13" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="14" spans="1:15">
+      <c r="A14" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B14">
+      <c r="B14" s="2">
         <v>13</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="4">
         <v>1.1781399176954725</v>
       </c>
-      <c r="D14">
+      <c r="D14" s="2">
         <v>0.14299999999999999</v>
       </c>
-      <c r="E14">
+      <c r="E14" s="2">
         <v>0.98099999999999998</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="2">
         <v>1.0209999999999999</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="2">
         <v>10</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="2">
         <v>1000</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="2">
         <v>295</v>
       </c>
-      <c r="J14">
-        <v>8</v>
-      </c>
-      <c r="K14" s="1">
+      <c r="J14" s="2">
+        <v>8</v>
+      </c>
+      <c r="K14" s="3">
         <v>39000</v>
       </c>
-      <c r="O14">
+      <c r="L14" s="2"/>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+      <c r="O14" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:15">
+      <c r="A15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="2">
         <v>14</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="2">
         <v>0.2</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="2">
         <v>0.126</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="2">
         <v>0.98099999999999998</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="2">
         <v>1.0209999999999999</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="2">
         <v>10</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="2">
         <v>1000</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="2">
         <v>257</v>
       </c>
-      <c r="J15">
-        <v>8</v>
-      </c>
-      <c r="K15" s="1">
+      <c r="J15" s="2">
+        <v>8</v>
+      </c>
+      <c r="K15" s="3">
         <v>64000</v>
       </c>
-      <c r="O15">
+      <c r="L15" s="2"/>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+      <c r="O15" s="2">
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:15">
+      <c r="A16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B16">
+      <c r="B16" s="2">
         <v>15</v>
       </c>
-      <c r="C16">
-        <v>16.95</v>
-      </c>
-      <c r="D16">
-        <v>0.68</v>
-      </c>
-      <c r="E16">
+      <c r="C16" s="2">
+        <v>12</v>
+      </c>
+      <c r="D16" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E16" s="2">
         <v>0.98599999999999999</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="2">
         <v>1.026</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="2">
         <v>100</v>
       </c>
-      <c r="J16">
-        <v>8</v>
-      </c>
-      <c r="K16" s="1">
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2">
+        <v>8</v>
+      </c>
+      <c r="K16" s="3">
         <v>5500</v>
       </c>
-      <c r="L16">
+      <c r="L16" s="2">
         <v>80</v>
       </c>
-      <c r="M16">
+      <c r="M16" s="2">
         <v>120</v>
       </c>
-      <c r="N16">
+      <c r="N16" s="2">
         <v>100</v>
       </c>
-      <c r="O16">
+      <c r="O16" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:15">
+      <c r="A17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="2">
         <v>16</v>
       </c>
-      <c r="C17">
-        <v>11.260000000000002</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="2">
+        <v>9.5500000000000007</v>
+      </c>
+      <c r="D17" s="2">
         <v>0.26</v>
       </c>
-      <c r="E17">
+      <c r="E17" s="2">
         <v>0.98</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="2">
         <v>1.02</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="2">
         <v>100</v>
       </c>
-      <c r="J17">
-        <v>8</v>
-      </c>
-      <c r="K17" s="1">
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2">
+        <v>8</v>
+      </c>
+      <c r="K17" s="3">
         <v>7300</v>
       </c>
-      <c r="L17">
+      <c r="L17" s="2">
         <v>80</v>
       </c>
-      <c r="M17">
+      <c r="M17" s="2">
         <v>120</v>
       </c>
-      <c r="N17">
+      <c r="N17" s="2">
         <v>100</v>
       </c>
-      <c r="O17">
+      <c r="O17" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:15">
+      <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>17</v>
       </c>
-      <c r="C18">
-        <v>3.42</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="2">
+        <v>2.67</v>
+      </c>
+      <c r="D18" s="2">
         <v>0.27</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>0.80800000000000005</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>0.85499999999999998</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>100</v>
       </c>
-      <c r="J18">
-        <v>8</v>
-      </c>
-      <c r="L18">
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2">
+        <v>8</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="2">
         <v>80</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="2">
         <v>120</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="2">
         <v>100</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:15">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="2">
         <v>18</v>
       </c>
-      <c r="C19">
-        <v>3.59</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="2">
+        <v>4.32</v>
+      </c>
+      <c r="D19" s="2">
         <v>0.38500000000000001</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="2">
         <v>0.98</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="2">
         <v>1.02</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="2">
         <v>100</v>
       </c>
-      <c r="J19">
-        <v>8</v>
-      </c>
-      <c r="K19" s="1">
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2">
+        <v>8</v>
+      </c>
+      <c r="K19" s="3">
         <v>2200</v>
       </c>
-      <c r="L19">
+      <c r="L19" s="2">
         <v>80</v>
       </c>
-      <c r="M19">
+      <c r="M19" s="2">
         <v>120</v>
       </c>
-      <c r="N19">
+      <c r="N19" s="2">
         <v>100</v>
       </c>
-      <c r="O19">
+      <c r="O19" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:15">
+      <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="2">
         <v>19</v>
       </c>
-      <c r="C20">
-        <v>11.6</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="2">
+        <v>8.6199999999999992</v>
+      </c>
+      <c r="D20" s="2">
         <v>0.373</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="2">
         <v>0.97</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="2">
         <v>1.03</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="2">
         <v>100</v>
       </c>
-      <c r="J20">
-        <v>8</v>
-      </c>
-      <c r="L20">
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2">
+        <v>8</v>
+      </c>
+      <c r="K20" s="3"/>
+      <c r="L20" s="2">
         <v>80</v>
       </c>
-      <c r="M20">
+      <c r="M20" s="2">
         <v>120</v>
       </c>
-      <c r="N20">
+      <c r="N20" s="2">
         <v>100</v>
       </c>
-      <c r="O20">
+      <c r="O20" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:15">
+      <c r="A21" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="2">
         <v>20</v>
       </c>
-      <c r="C21">
-        <v>10.530000000000001</v>
-      </c>
-      <c r="D21">
+      <c r="C21" s="2">
+        <v>7.71</v>
+      </c>
+      <c r="D21" s="2">
         <v>0.29399999999999998</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="2">
         <v>0.96030000000000004</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="2">
         <v>1.0197000000000001</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="2">
         <v>100</v>
       </c>
-      <c r="J21">
-        <v>8</v>
-      </c>
-      <c r="L21">
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2">
+        <v>8</v>
+      </c>
+      <c r="K21" s="3"/>
+      <c r="L21" s="2">
         <v>80</v>
       </c>
-      <c r="M21">
+      <c r="M21" s="2">
         <v>120</v>
       </c>
-      <c r="N21">
+      <c r="N21" s="2">
         <v>100</v>
       </c>
-      <c r="O21">
+      <c r="O21" s="2">
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15">
       <c r="K24"/>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15">
       <c r="K25"/>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15">
       <c r="K26"/>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15">
       <c r="K27"/>
     </row>
   </sheetData>

</xml_diff>